<commit_message>
saque el cp a texto
</commit_message>
<xml_diff>
--- a/LBM.xlsx
+++ b/LBM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lmenghi\Desktop\RUTEO\SALUD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0F0D74A3-5722-405A-B1EF-A61D0545165F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6368D868-4508-430A-85B9-8055FB2E086B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{A7CB6BBD-62E7-4B8B-968D-88CBEA9AFE12}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{3BBEF559-4E8A-4A35-9CFD-D870795C93BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="105">
   <si>
     <t>Equipo</t>
   </si>
@@ -174,7 +174,76 @@
     <t>Calidad – GEO</t>
   </si>
   <si>
-    <t>1229601266</t>
+    <t>1229655860</t>
+  </si>
+  <si>
+    <t>LBM</t>
+  </si>
+  <si>
+    <t>AV. SANTA FE 2534</t>
+  </si>
+  <si>
+    <t>CAPITAL FEDERAL</t>
+  </si>
+  <si>
+    <t>Capital Federal</t>
+  </si>
+  <si>
+    <t>0800</t>
+  </si>
+  <si>
+    <t>2000</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>MARKEN TIME CRITICAL EXPRESS S.A.</t>
+  </si>
+  <si>
+    <t>620X37567625</t>
+  </si>
+  <si>
+    <t>000000001229655860</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>1425</t>
+  </si>
+  <si>
+    <t>Envio</t>
+  </si>
+  <si>
+    <t>20251127</t>
+  </si>
+  <si>
+    <t>BIO SPX REFRIGERATED -DOMESTIC-  2ºC/8ºC</t>
+  </si>
+  <si>
+    <t>Retirado</t>
+  </si>
+  <si>
+    <t>BUE</t>
+  </si>
+  <si>
+    <t>CONTENEDOR EN DESTINO</t>
+  </si>
+  <si>
+    <t>AR</t>
+  </si>
+  <si>
+    <t>Dist. de Muestras biológicas / genét AMB</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1229659459</t>
   </si>
   <si>
     <t>LABORATORIO BIOQUIMICA MEDICA</t>
@@ -183,115 +252,67 @@
     <t>AV SANTA FE 2534 PISO 1</t>
   </si>
   <si>
-    <t>CAPITAL FEDERAL</t>
-  </si>
-  <si>
-    <t>Capital Federal</t>
-  </si>
-  <si>
-    <t>0800</t>
-  </si>
-  <si>
-    <t>2000</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>Ocasa Inc (Miami)</t>
   </si>
   <si>
-    <t>PK2AWRW59874</t>
-  </si>
-  <si>
-    <t>000000001229601266</t>
+    <t>PK2I6XJ60852</t>
+  </si>
+  <si>
+    <t>000000001229659459</t>
   </si>
   <si>
     <t>77</t>
   </si>
   <si>
-    <t>1425</t>
-  </si>
-  <si>
     <t xml:space="preserve"> HUMAN BIOLOGICAL SUBSTANCE - CATEGO RY B UN3373</t>
   </si>
   <si>
-    <t>Envio</t>
-  </si>
-  <si>
-    <t>20251126</t>
-  </si>
-  <si>
     <t>HUMAN BIOLOGICAL SUBSTANCES CAT B-UN3373</t>
   </si>
   <si>
-    <t>Retirado</t>
-  </si>
-  <si>
-    <t>BUE</t>
-  </si>
-  <si>
     <t>PENDIENTE DE DISTRIBUCION</t>
   </si>
   <si>
-    <t>AR</t>
-  </si>
-  <si>
     <t>Envío de muestras biológ. y genét. - REF</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>1229601583</t>
-  </si>
-  <si>
-    <t>PK2E6GR60506</t>
-  </si>
-  <si>
-    <t>000000001229601583</t>
-  </si>
-  <si>
-    <t>1229601587</t>
-  </si>
-  <si>
-    <t>PK2EKGP60514</t>
-  </si>
-  <si>
-    <t>000000001229601587</t>
-  </si>
-  <si>
-    <t>1229601589</t>
-  </si>
-  <si>
-    <t>PK2RAAZ60512</t>
-  </si>
-  <si>
-    <t>000000001229601589</t>
-  </si>
-  <si>
-    <t>1229601752</t>
-  </si>
-  <si>
-    <t>PK2M9CH60403</t>
-  </si>
-  <si>
-    <t>000000001229601752</t>
-  </si>
-  <si>
-    <t>1229601754</t>
-  </si>
-  <si>
-    <t>PK2MPZM60405</t>
-  </si>
-  <si>
-    <t>000000001229601754</t>
-  </si>
-  <si>
-    <t>1229601821</t>
+    <t>1229664579</t>
+  </si>
+  <si>
+    <t>PK2BNRK60914</t>
+  </si>
+  <si>
+    <t>000000001229664579</t>
+  </si>
+  <si>
+    <t>1229665340</t>
+  </si>
+  <si>
+    <t>PK24B7M61035</t>
+  </si>
+  <si>
+    <t>000000001229665340</t>
+  </si>
+  <si>
+    <t>1229665805</t>
+  </si>
+  <si>
+    <t>PK2WLE161037</t>
+  </si>
+  <si>
+    <t>000000001229665805</t>
+  </si>
+  <si>
+    <t>1229666564</t>
+  </si>
+  <si>
+    <t>PK2ELNW59879</t>
+  </si>
+  <si>
+    <t>000000001229666564</t>
+  </si>
+  <si>
+    <t>1229669643</t>
   </si>
   <si>
     <t>AV SANTA FE 2534 PISO 1-1425</t>
@@ -300,49 +321,22 @@
     <t>54-114-826-8783</t>
   </si>
   <si>
-    <t>M7744119</t>
-  </si>
-  <si>
-    <t>000000001229601821</t>
+    <t>M7744117</t>
+  </si>
+  <si>
+    <t>000000001229669643</t>
   </si>
   <si>
     <t xml:space="preserve"> HUMAN BIOLOGICAL SUBSTANCE                 CATEGORY B UN3373</t>
   </si>
   <si>
-    <t>1229601823</t>
-  </si>
-  <si>
-    <t>PK2KD6H60605</t>
-  </si>
-  <si>
-    <t>000000001229601823</t>
-  </si>
-  <si>
-    <t>1229601826</t>
-  </si>
-  <si>
-    <t>PK2SBBW59779</t>
-  </si>
-  <si>
-    <t>000000001229601826</t>
-  </si>
-  <si>
-    <t>1229601964</t>
-  </si>
-  <si>
-    <t>LABORATORIO BIOQUIMICA</t>
-  </si>
-  <si>
-    <t>AV. SANTA FE 2534</t>
-  </si>
-  <si>
-    <t>Ocasa Inc (New York)</t>
-  </si>
-  <si>
-    <t>B1648496</t>
-  </si>
-  <si>
-    <t>000000001229601964</t>
+    <t>1229669872</t>
+  </si>
+  <si>
+    <t>PK2BJAT60570</t>
+  </si>
+  <si>
+    <t>000000001229669872</t>
   </si>
 </sst>
 </file>
@@ -1215,8 +1209,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6ED8C36-7231-49B2-8187-16F71B036DB4}">
-  <dimension ref="A1:AX11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4441494-04FF-42A0-8E19-C67FF257F2A4}">
+  <dimension ref="A1:AX9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1241,7 +1235,7 @@
     <col min="15" max="15" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="36.7109375" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="6.5703125" bestFit="1" customWidth="1"/>
@@ -1265,7 +1259,7 @@
     <col min="40" max="40" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="28.28515625" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="12" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="35.5703125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="36.140625" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="45" max="46" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="47" max="47" width="15.85546875" bestFit="1" customWidth="1"/>
@@ -1457,10 +1451,10 @@
         <v>57</v>
       </c>
       <c r="N2" s="3">
-        <v>4.8000000000000001E-2</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="O2" s="3">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>58</v>
@@ -1471,7 +1465,7 @@
       </c>
       <c r="S2" s="1"/>
       <c r="T2" s="4">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="U2" s="1"/>
       <c r="V2" s="1"/>
@@ -1494,37 +1488,35 @@
       <c r="AG2" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="AH2" s="1" t="s">
+      <c r="AH2" s="1"/>
+      <c r="AI2" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AI2" s="1" t="s">
+      <c r="AJ2" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="AJ2" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="AK2" s="1"/>
       <c r="AL2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AM2" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="AM2" s="1" t="s">
+      <c r="AN2" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="AN2" s="1" t="s">
+      <c r="AO2" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AO2" s="1" t="s">
+      <c r="AP2" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AP2" s="1" t="s">
+      <c r="AQ2" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="AQ2" s="1" t="s">
-        <v>72</v>
       </c>
       <c r="AR2" s="1"/>
       <c r="AS2" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AT2" s="1"/>
       <c r="AU2" s="1"/>
@@ -1534,13 +1526,13 @@
     </row>
     <row r="3" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>52</v>
+        <v>75</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
@@ -1573,7 +1565,7 @@
       </c>
       <c r="Q3" s="1"/>
       <c r="R3" s="1" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="S3" s="1"/>
       <c r="T3" s="4">
@@ -1584,53 +1576,53 @@
       <c r="W3" s="1"/>
       <c r="X3" s="1"/>
       <c r="Y3" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="Z3" s="1"/>
       <c r="AA3" s="1"/>
       <c r="AB3" s="1"/>
       <c r="AC3" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="AD3" s="1"/>
       <c r="AE3" s="1" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="AF3" s="1"/>
       <c r="AG3" s="1" t="s">
         <v>63</v>
       </c>
       <c r="AH3" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AI3" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AI3" s="1" t="s">
+      <c r="AJ3" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="AJ3" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="AK3" s="1"/>
       <c r="AL3" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AM3" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="AM3" s="1" t="s">
+      <c r="AN3" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="AN3" s="1" t="s">
-        <v>69</v>
-      </c>
       <c r="AO3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP3" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AP3" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="AQ3" s="1" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="AR3" s="1"/>
       <c r="AS3" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AT3" s="1"/>
       <c r="AU3" s="1"/>
@@ -1640,13 +1632,13 @@
     </row>
     <row r="4" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>52</v>
+        <v>75</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
@@ -1679,7 +1671,7 @@
       </c>
       <c r="Q4" s="1"/>
       <c r="R4" s="1" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="S4" s="1"/>
       <c r="T4" s="4">
@@ -1690,53 +1682,53 @@
       <c r="W4" s="1"/>
       <c r="X4" s="1"/>
       <c r="Y4" s="1" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="Z4" s="1"/>
       <c r="AA4" s="1"/>
       <c r="AB4" s="1"/>
       <c r="AC4" s="1" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="AD4" s="1"/>
       <c r="AE4" s="1" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="AF4" s="1"/>
       <c r="AG4" s="1" t="s">
         <v>63</v>
       </c>
       <c r="AH4" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AI4" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AI4" s="1" t="s">
+      <c r="AJ4" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="AJ4" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="AK4" s="1"/>
       <c r="AL4" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AM4" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="AM4" s="1" t="s">
+      <c r="AN4" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="AN4" s="1" t="s">
-        <v>69</v>
-      </c>
       <c r="AO4" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP4" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AP4" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="AQ4" s="1" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="AR4" s="1"/>
       <c r="AS4" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AT4" s="1"/>
       <c r="AU4" s="1"/>
@@ -1746,13 +1738,13 @@
     </row>
     <row r="5" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>52</v>
+        <v>75</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
@@ -1785,64 +1777,64 @@
       </c>
       <c r="Q5" s="1"/>
       <c r="R5" s="1" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="S5" s="1"/>
       <c r="T5" s="4">
-        <v>0.01</v>
+        <v>0.1</v>
       </c>
       <c r="U5" s="1"/>
       <c r="V5" s="1"/>
       <c r="W5" s="1"/>
       <c r="X5" s="1"/>
       <c r="Y5" s="1" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="Z5" s="1"/>
       <c r="AA5" s="1"/>
       <c r="AB5" s="1"/>
       <c r="AC5" s="1" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="AD5" s="1"/>
       <c r="AE5" s="1" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="AF5" s="1"/>
       <c r="AG5" s="1" t="s">
         <v>63</v>
       </c>
       <c r="AH5" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AI5" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AI5" s="1" t="s">
+      <c r="AJ5" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="AJ5" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="AK5" s="1"/>
       <c r="AL5" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AM5" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="AM5" s="1" t="s">
+      <c r="AN5" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="AN5" s="1" t="s">
-        <v>69</v>
-      </c>
       <c r="AO5" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP5" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AP5" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="AQ5" s="1" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="AR5" s="1"/>
       <c r="AS5" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AT5" s="1"/>
       <c r="AU5" s="1"/>
@@ -1852,13 +1844,13 @@
     </row>
     <row r="6" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>52</v>
+        <v>75</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
@@ -1891,7 +1883,7 @@
       </c>
       <c r="Q6" s="1"/>
       <c r="R6" s="1" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="S6" s="1"/>
       <c r="T6" s="4">
@@ -1902,53 +1894,53 @@
       <c r="W6" s="1"/>
       <c r="X6" s="1"/>
       <c r="Y6" s="1" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="Z6" s="1"/>
       <c r="AA6" s="1"/>
       <c r="AB6" s="1"/>
       <c r="AC6" s="1" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="AD6" s="1"/>
       <c r="AE6" s="1" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="AF6" s="1"/>
       <c r="AG6" s="1" t="s">
         <v>63</v>
       </c>
       <c r="AH6" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AI6" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AI6" s="1" t="s">
+      <c r="AJ6" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="AJ6" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="AK6" s="1"/>
       <c r="AL6" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AM6" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="AM6" s="1" t="s">
+      <c r="AN6" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="AN6" s="1" t="s">
-        <v>69</v>
-      </c>
       <c r="AO6" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP6" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AP6" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="AQ6" s="1" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="AR6" s="1"/>
       <c r="AS6" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AT6" s="1"/>
       <c r="AU6" s="1"/>
@@ -1958,13 +1950,13 @@
     </row>
     <row r="7" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>52</v>
+        <v>75</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
@@ -1987,7 +1979,7 @@
         <v>57</v>
       </c>
       <c r="N7" s="3">
-        <v>4.8000000000000001E-2</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="O7" s="3">
         <v>3</v>
@@ -1997,7 +1989,7 @@
       </c>
       <c r="Q7" s="1"/>
       <c r="R7" s="1" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="S7" s="1"/>
       <c r="T7" s="4">
@@ -2008,53 +2000,51 @@
       <c r="W7" s="1"/>
       <c r="X7" s="1"/>
       <c r="Y7" s="1" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="Z7" s="1"/>
       <c r="AA7" s="1"/>
       <c r="AB7" s="1"/>
       <c r="AC7" s="1" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="AD7" s="1"/>
       <c r="AE7" s="1" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="AF7" s="1"/>
       <c r="AG7" s="1" t="s">
         <v>63</v>
       </c>
       <c r="AH7" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AI7" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AI7" s="1" t="s">
+      <c r="AJ7" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="AJ7" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="AK7" s="1"/>
       <c r="AL7" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AM7" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AM7" s="1"/>
+      <c r="AN7" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="AN7" s="1" t="s">
-        <v>69</v>
-      </c>
       <c r="AO7" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP7" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AP7" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="AQ7" s="1" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="AR7" s="1"/>
       <c r="AS7" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AT7" s="1"/>
       <c r="AU7" s="1"/>
@@ -2064,13 +2054,13 @@
     </row>
     <row r="8" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
@@ -2093,7 +2083,7 @@
         <v>57</v>
       </c>
       <c r="N8" s="3">
-        <v>4.8000000000000001E-2</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="O8" s="3">
         <v>3</v>
@@ -2103,7 +2093,7 @@
       </c>
       <c r="Q8" s="1"/>
       <c r="R8" s="1" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="S8" s="1"/>
       <c r="T8" s="4">
@@ -2112,57 +2102,57 @@
       <c r="U8" s="1"/>
       <c r="V8" s="1"/>
       <c r="W8" s="1" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="X8" s="1"/>
       <c r="Y8" s="1" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="Z8" s="1"/>
       <c r="AA8" s="1"/>
       <c r="AB8" s="1"/>
       <c r="AC8" s="1" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="AD8" s="1"/>
       <c r="AE8" s="1" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="AF8" s="1"/>
       <c r="AG8" s="1" t="s">
         <v>63</v>
       </c>
       <c r="AH8" s="1" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="AI8" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AJ8" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="AJ8" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="AK8" s="1"/>
       <c r="AL8" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AM8" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="AM8" s="1" t="s">
+      <c r="AN8" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="AN8" s="1" t="s">
-        <v>69</v>
-      </c>
       <c r="AO8" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP8" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AP8" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="AQ8" s="1" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="AR8" s="1"/>
       <c r="AS8" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AT8" s="1"/>
       <c r="AU8" s="1"/>
@@ -2172,13 +2162,13 @@
     </row>
     <row r="9" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>52</v>
+        <v>75</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1" t="s">
@@ -2201,7 +2191,7 @@
         <v>57</v>
       </c>
       <c r="N9" s="3">
-        <v>4.8000000000000001E-2</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="O9" s="3">
         <v>3</v>
@@ -2211,7 +2201,7 @@
       </c>
       <c r="Q9" s="1"/>
       <c r="R9" s="1" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="S9" s="1"/>
       <c r="T9" s="4">
@@ -2222,265 +2212,59 @@
       <c r="W9" s="1"/>
       <c r="X9" s="1"/>
       <c r="Y9" s="1" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="Z9" s="1"/>
       <c r="AA9" s="1"/>
       <c r="AB9" s="1"/>
       <c r="AC9" s="1" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="AD9" s="1"/>
       <c r="AE9" s="1" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="AF9" s="1"/>
       <c r="AG9" s="1" t="s">
         <v>63</v>
       </c>
       <c r="AH9" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AI9" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AI9" s="1" t="s">
+      <c r="AJ9" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="AJ9" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="AK9" s="1"/>
       <c r="AL9" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AM9" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="AM9" s="1" t="s">
+      <c r="AN9" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="AN9" s="1" t="s">
-        <v>69</v>
-      </c>
       <c r="AO9" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP9" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AP9" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="AQ9" s="1" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="AR9" s="1"/>
       <c r="AS9" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AT9" s="1"/>
       <c r="AU9" s="1"/>
       <c r="AV9" s="1"/>
       <c r="AW9" s="1"/>
       <c r="AX9" s="1"/>
-    </row>
-    <row r="10" spans="1:50" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="N10" s="3">
-        <v>4.8000000000000001E-2</v>
-      </c>
-      <c r="O10" s="3">
-        <v>3</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="S10" s="1"/>
-      <c r="T10" s="4">
-        <v>0.01</v>
-      </c>
-      <c r="U10" s="1"/>
-      <c r="V10" s="1"/>
-      <c r="W10" s="1"/>
-      <c r="X10" s="1"/>
-      <c r="Y10" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="Z10" s="1"/>
-      <c r="AA10" s="1"/>
-      <c r="AB10" s="1"/>
-      <c r="AC10" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="AD10" s="1"/>
-      <c r="AE10" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="AF10" s="1"/>
-      <c r="AG10" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="AH10" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="AI10" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="AJ10" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="AK10" s="1"/>
-      <c r="AL10" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AM10" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="AN10" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AO10" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="AP10" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AQ10" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="AR10" s="1"/>
-      <c r="AS10" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="AT10" s="1"/>
-      <c r="AU10" s="1"/>
-      <c r="AV10" s="1"/>
-      <c r="AW10" s="1"/>
-      <c r="AX10" s="1"/>
-    </row>
-    <row r="11" spans="1:50" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="N11" s="3">
-        <v>4.8000000000000001E-2</v>
-      </c>
-      <c r="O11" s="3">
-        <v>3</v>
-      </c>
-      <c r="P11" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q11" s="1"/>
-      <c r="R11" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="S11" s="1"/>
-      <c r="T11" s="4">
-        <v>0.01</v>
-      </c>
-      <c r="U11" s="1"/>
-      <c r="V11" s="1"/>
-      <c r="W11" s="1"/>
-      <c r="X11" s="1"/>
-      <c r="Y11" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="Z11" s="1"/>
-      <c r="AA11" s="1"/>
-      <c r="AB11" s="1"/>
-      <c r="AC11" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="AD11" s="1"/>
-      <c r="AE11" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="AF11" s="1"/>
-      <c r="AG11" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="AH11" s="1"/>
-      <c r="AI11" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="AJ11" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="AK11" s="1"/>
-      <c r="AL11" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AM11" s="1"/>
-      <c r="AN11" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AO11" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="AP11" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AQ11" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="AR11" s="1"/>
-      <c r="AS11" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="AT11" s="1"/>
-      <c r="AU11" s="1"/>
-      <c r="AV11" s="1"/>
-      <c r="AW11" s="1"/>
-      <c r="AX11" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2489,7 +2273,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A56F0C6-A0A7-4B5A-A624-50D47A747C47}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0840343C-9FB0-42D9-B1C0-646DC594BCAC}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2501,7 +2285,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34D42C27-089A-4B8D-877A-1229977471F4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F06B36AB-8D40-4191-B6BF-7E68A6F36187}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>